<commit_message>
manual uploading 2021/07/2 8:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/BMZ.xlsx
+++ b/src/algorithms/plan_fact_module/BMZ.xlsx
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="B333" sqref="B333"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
manual dislocation uploading 2021/07/26 20:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/BMZ.xlsx
+++ b/src/algorithms/plan_fact_module/BMZ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="9">
   <si>
     <t>CarAmount</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>МЕДЬ</t>
+  </si>
+  <si>
+    <t>Новороссийск (эксп.)</t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -146,6 +149,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal 3" xfId="5"/>
@@ -432,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E363"/>
+  <dimension ref="A1:F363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +451,7 @@
     <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -464,9 +468,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>44378</v>
+        <v>44409</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -481,9 +485,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44379</v>
+        <v>44410</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -498,12 +502,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>44380</v>
+        <v>44411</v>
       </c>
       <c r="B4" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -515,9 +519,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>44381</v>
+        <v>44412</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -532,9 +536,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>44382</v>
+        <v>44413</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -549,9 +553,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>44383</v>
+        <v>44414</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -566,9 +570,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>44384</v>
+        <v>44415</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -583,9 +587,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>44385</v>
+        <v>44416</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -600,12 +604,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>44386</v>
+        <v>44417</v>
       </c>
       <c r="B10" s="1">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -616,10 +620,11 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>44387</v>
+        <v>44418</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -633,10 +638,11 @@
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>44388</v>
+        <v>44419</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -650,10 +656,11 @@
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>44389</v>
+        <v>44420</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -667,10 +674,11 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>44390</v>
+        <v>44421</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -684,10 +692,11 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>44391</v>
+        <v>44422</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -701,10 +710,11 @@
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>44392</v>
+        <v>44423</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -718,13 +728,14 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>44393</v>
+        <v>44424</v>
       </c>
       <c r="B17" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -735,10 +746,11 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>44394</v>
+        <v>44425</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -752,10 +764,11 @@
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>44395</v>
+        <v>44426</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -769,31 +782,33 @@
       <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>44396</v>
+        <v>44427</v>
       </c>
       <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>44428</v>
+      </c>
+      <c r="B21" s="1">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>44397</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
@@ -804,9 +819,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>44398</v>
+        <v>44429</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -821,9 +836,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>44399</v>
+        <v>44430</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -838,9 +853,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>44400</v>
+        <v>44431</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -855,9 +870,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>44401</v>
+        <v>44432</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -872,9 +887,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>44402</v>
+        <v>44433</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -889,12 +904,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>44403</v>
+        <v>44434</v>
       </c>
       <c r="B27" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -906,12 +921,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>44404</v>
+        <v>44435</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -923,9 +938,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>44405</v>
+        <v>44436</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -940,9 +955,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>44406</v>
+        <v>44437</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -957,12 +972,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>44407</v>
+        <v>44438</v>
       </c>
       <c r="B31" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -974,12 +989,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>44408</v>
+        <v>44439</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -992,9 +1007,21 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1"/>
-      <c r="E33" s="2"/>
+      <c r="A33" s="3">
+        <v>44425</v>
+      </c>
+      <c r="B33" s="1">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>

</xml_diff>

<commit_message>
manual dislocation uploading 2021/08/21 13:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/BMZ.xlsx
+++ b/src/algorithms/plan_fact_module/BMZ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="9600" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="8">
   <si>
     <t>CarAmount</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>МЕДЬ</t>
-  </si>
-  <si>
-    <t>Новороссийск (эксп.)</t>
   </si>
 </sst>
 </file>
@@ -438,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B2:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +467,7 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>44409</v>
+        <v>44440</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -487,7 +484,7 @@
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44410</v>
+        <v>44441</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -504,7 +501,7 @@
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>44411</v>
+        <v>44442</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -521,7 +518,7 @@
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>44412</v>
+        <v>44443</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -538,7 +535,7 @@
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>44413</v>
+        <v>44444</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -555,10 +552,10 @@
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>44414</v>
+        <v>44445</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -572,7 +569,7 @@
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>44415</v>
+        <v>44446</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -589,7 +586,7 @@
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>44416</v>
+        <v>44447</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -606,10 +603,10 @@
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>44417</v>
+        <v>44448</v>
       </c>
       <c r="B10" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -624,10 +621,10 @@
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>44418</v>
+        <v>44449</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -642,7 +639,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>44419</v>
+        <v>44450</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -660,7 +657,7 @@
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>44420</v>
+        <v>44451</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -678,7 +675,7 @@
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>44421</v>
+        <v>44452</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -696,7 +693,7 @@
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>44422</v>
+        <v>44453</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -714,7 +711,7 @@
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>44423</v>
+        <v>44454</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -732,10 +729,10 @@
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>44424</v>
+        <v>44455</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -750,7 +747,7 @@
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>44425</v>
+        <v>44456</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -768,7 +765,7 @@
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>44426</v>
+        <v>44457</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -786,7 +783,7 @@
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>44427</v>
+        <v>44458</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -804,10 +801,10 @@
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>44428</v>
+        <v>44459</v>
       </c>
       <c r="B21" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>44429</v>
+        <v>44460</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -838,7 +835,7 @@
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>44430</v>
+        <v>44461</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -855,10 +852,10 @@
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>44431</v>
+        <v>44462</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -872,7 +869,7 @@
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>44432</v>
+        <v>44463</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -889,7 +886,7 @@
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>44433</v>
+        <v>44464</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -906,7 +903,7 @@
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>44434</v>
+        <v>44465</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -923,10 +920,10 @@
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>44435</v>
+        <v>44466</v>
       </c>
       <c r="B28" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -940,7 +937,7 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>44436</v>
+        <v>44467</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -957,10 +954,10 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>44437</v>
+        <v>44468</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -974,7 +971,7 @@
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>44438</v>
+        <v>44469</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -990,38 +987,15 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>44439</v>
-      </c>
-      <c r="B32" s="1">
-        <v>20</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="1"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
-        <v>44425</v>
-      </c>
-      <c r="B33" s="1">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="1"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>

</xml_diff>

<commit_message>
manual dislocation uploading 2021/11/06 21:00
</commit_message>
<xml_diff>
--- a/src/algorithms/plan_fact_module/BMZ.xlsx
+++ b/src/algorithms/plan_fact_module/BMZ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9600" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="8">
   <si>
     <t>CarAmount</t>
   </si>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B2:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +467,7 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>44440</v>
+        <v>44470</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44441</v>
+        <v>44471</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -501,7 +501,7 @@
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>44442</v>
+        <v>44472</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>44443</v>
+        <v>44473</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>44444</v>
+        <v>44474</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -552,10 +552,10 @@
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>44445</v>
+        <v>44475</v>
       </c>
       <c r="B7" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>44446</v>
+        <v>44476</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>44447</v>
+        <v>44477</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>44448</v>
+        <v>44478</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>44449</v>
+        <v>44479</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>44450</v>
+        <v>44480</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>44451</v>
+        <v>44481</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>44452</v>
+        <v>44482</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>44453</v>
+        <v>44483</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>44454</v>
+        <v>44484</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>44455</v>
+        <v>44485</v>
       </c>
       <c r="B17" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>44456</v>
+        <v>44486</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>44457</v>
+        <v>44487</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>44458</v>
+        <v>44488</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>44459</v>
+        <v>44489</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>44460</v>
+        <v>44490</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>44461</v>
+        <v>44491</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -852,10 +852,10 @@
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>44462</v>
+        <v>44492</v>
       </c>
       <c r="B24" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>44463</v>
+        <v>44493</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>44464</v>
+        <v>44494</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>44465</v>
+        <v>44495</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>44466</v>
+        <v>44496</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>44467</v>
+        <v>44497</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>44468</v>
+        <v>44498</v>
       </c>
       <c r="B30" s="1">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>44469</v>
+        <v>44499</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -987,160 +987,531 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1"/>
-      <c r="E32" s="2"/>
+      <c r="A32" s="3">
+        <v>44500</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="2"/>
+      <c r="A33" s="3">
+        <v>44501</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="1"/>
-      <c r="E34" s="2"/>
+      <c r="A34" s="3">
+        <v>44502</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="3">
+        <v>44503</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="1"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="3">
+        <v>44504</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="1"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="3">
+        <v>44505</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="1"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="3">
+        <v>44506</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="1"/>
-      <c r="E39" s="2"/>
+      <c r="A39" s="3">
+        <v>44507</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="1"/>
-      <c r="E40" s="2"/>
+      <c r="A40" s="3">
+        <v>44508</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="1"/>
-      <c r="E41" s="2"/>
+      <c r="A41" s="3">
+        <v>44509</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-      <c r="B42" s="1"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="3">
+        <v>44510</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="1"/>
-      <c r="E43" s="2"/>
+      <c r="A43" s="3">
+        <v>44511</v>
+      </c>
+      <c r="B43" s="1">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="1"/>
-      <c r="E44" s="2"/>
+      <c r="A44" s="3">
+        <v>44512</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-      <c r="B45" s="1"/>
-      <c r="E45" s="2"/>
+      <c r="A45" s="3">
+        <v>44513</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="1"/>
-      <c r="E46" s="2"/>
+      <c r="A46" s="3">
+        <v>44514</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="1"/>
-      <c r="E47" s="2"/>
+      <c r="A47" s="3">
+        <v>44515</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="1"/>
-      <c r="E48" s="2"/>
+      <c r="A48" s="3">
+        <v>44516</v>
+      </c>
+      <c r="B48" s="1">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="1"/>
-      <c r="E49" s="2"/>
+      <c r="A49" s="3">
+        <v>44517</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="1"/>
-      <c r="E50" s="2"/>
+      <c r="A50" s="3">
+        <v>44518</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="1"/>
-      <c r="E51" s="2"/>
+      <c r="A51" s="3">
+        <v>44519</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="1"/>
-      <c r="E52" s="2"/>
+      <c r="A52" s="3">
+        <v>44520</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="1"/>
-      <c r="E53" s="2"/>
+      <c r="A53" s="3">
+        <v>44521</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A54" s="3"/>
-      <c r="B54" s="1"/>
-      <c r="E54" s="2"/>
+      <c r="A54" s="3">
+        <v>44522</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-      <c r="B55" s="1"/>
-      <c r="E55" s="2"/>
+      <c r="A55" s="3">
+        <v>44523</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="1"/>
-      <c r="E56" s="2"/>
+      <c r="A56" s="3">
+        <v>44524</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-      <c r="B57" s="1"/>
-      <c r="E57" s="2"/>
+      <c r="A57" s="3">
+        <v>44525</v>
+      </c>
+      <c r="B57" s="1">
+        <v>15</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
-      <c r="B58" s="1"/>
-      <c r="E58" s="2"/>
+      <c r="A58" s="3">
+        <v>44526</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-      <c r="B59" s="1"/>
-      <c r="E59" s="2"/>
+      <c r="A59" s="3">
+        <v>44527</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="1"/>
-      <c r="E60" s="2"/>
+      <c r="A60" s="3">
+        <v>44528</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-      <c r="B61" s="1"/>
-      <c r="E61" s="2"/>
+      <c r="A61" s="3">
+        <v>44529</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="1"/>
-      <c r="E62" s="2"/>
+      <c r="A62" s="3">
+        <v>44530</v>
+      </c>
+      <c r="B62" s="1">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>

</xml_diff>